<commit_message>
JetStream 2 for iPhone 7
</commit_message>
<xml_diff>
--- a/geekbench/geekbench.xlsx
+++ b/geekbench/geekbench.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="222" documentId="13_ncr:1_{C05CC734-0992-4C88-AFA7-52482F562631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A14E7F77-72DD-4026-9BE3-6DC11D94A156}"/>
+  <xr:revisionPtr revIDLastSave="223" documentId="13_ncr:1_{C05CC734-0992-4C88-AFA7-52482F562631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{9D021925-485A-41DD-8883-2AF25CCFC59E}"/>
   <bookViews>
-    <workbookView xWindow="20040" yWindow="630" windowWidth="15975" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17385" yWindow="630" windowWidth="18630" windowHeight="17295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="2" r:id="rId1"/>
@@ -715,9 +715,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D653D24C-6F75-4FA8-B5E9-8831F728F129}">
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D34" sqref="D34"/>
+      <selection pane="topRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,6 +1611,9 @@
       <c r="M23" s="1"/>
       <c r="N23">
         <v>26491</v>
+      </c>
+      <c r="O23">
+        <v>81</v>
       </c>
       <c r="P23">
         <v>123</v>

</xml_diff>

<commit_message>
results for Raspberry Pi 3
</commit_message>
<xml_diff>
--- a/geekbench/geekbench.xlsx
+++ b/geekbench/geekbench.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D725ACE-1338-44B5-B25A-5695B2837711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B160B95F-1B8F-4229-8542-99946E4798F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="510" windowWidth="23010" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="22185" windowHeight="13395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="137">
   <si>
     <t>Neue Benchmarkliste</t>
   </si>
@@ -415,6 +415,27 @@
   </si>
   <si>
     <t>Cortex-A53</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - </t>
+  </si>
+  <si>
+    <t>MacBook Air 2020 M1</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>8 x 3200</t>
+  </si>
+  <si>
+    <t>7 core apple</t>
+  </si>
+  <si>
+    <t>iPad air 4</t>
+  </si>
+  <si>
+    <t>A14</t>
   </si>
 </sst>
 </file>
@@ -460,7 +481,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -493,14 +514,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -786,7 +811,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O4" sqref="O4"/>
+      <selection pane="topRight" activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,32 +837,32 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13" t="s">
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="13"/>
-      <c r="M2" s="12" t="s">
+      <c r="L2" s="14"/>
+      <c r="M2" s="13" t="s">
         <v>34</v>
       </c>
       <c r="N2" s="9"/>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12" t="s">
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="R2" s="12"/>
+      <c r="R2" s="13"/>
     </row>
     <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -874,7 +899,7 @@
       <c r="L3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="12"/>
+      <c r="M3" s="13"/>
       <c r="N3" s="3" t="s">
         <v>50</v>
       </c>
@@ -907,7 +932,7 @@
       <c r="B4" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>126</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -921,13 +946,19 @@
       <c r="J4" s="6"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="3">
+      <c r="M4" s="1">
+        <v>255</v>
+      </c>
+      <c r="N4" s="5">
         <v>155</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
-      <c r="Q4" s="14">
+      <c r="O4" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="P4" s="12">
+        <v>1.7</v>
+      </c>
+      <c r="Q4" s="16">
         <v>0.67800000000000005</v>
       </c>
       <c r="R4">
@@ -936,7 +967,9 @@
       <c r="S4">
         <v>1</v>
       </c>
-      <c r="T4" s="3"/>
+      <c r="T4" s="5">
+        <v>3631</v>
+      </c>
       <c r="U4" s="3">
         <v>125887</v>
       </c>
@@ -965,13 +998,26 @@
       <c r="M5" s="1">
         <v>1200</v>
       </c>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
+      <c r="N5">
+        <v>1586</v>
+      </c>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15">
+        <v>9.9</v>
+      </c>
+      <c r="Q5" s="15">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R5" s="15">
+        <v>8.4209999999999994</v>
+      </c>
+      <c r="S5" s="15">
+        <v>1.86</v>
+      </c>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15">
+        <v>22988</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
@@ -2189,7 +2235,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -2228,21 +2274,55 @@
       </c>
       <c r="M33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>131</v>
+      </c>
+      <c r="B34" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>134</v>
+      </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <v>238</v>
+      </c>
+      <c r="Q34">
+        <v>227</v>
+      </c>
+      <c r="S34">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>135</v>
+      </c>
+      <c r="B35" t="s">
+        <v>136</v>
+      </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35">
+        <v>57779</v>
+      </c>
+      <c r="S35">
+        <v>1188</v>
+      </c>
+      <c r="U35">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -2252,35 +2332,35 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -2328,16 +2408,16 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="13"/>
-      <c r="I2" s="12" t="s">
+      <c r="H2" s="14"/>
+      <c r="I2" s="13" t="s">
         <v>34</v>
       </c>
       <c r="J2" s="8"/>
@@ -2365,7 +2445,7 @@
       <c r="H3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="12"/>
+      <c r="I3" s="13"/>
       <c r="J3" s="3" t="s">
         <v>50</v>
       </c>

</xml_diff>